<commit_message>
Update energy run notebook with trde elasticities mods
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_se_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_se_calibrated.xlsx
@@ -621,85 +621,85 @@
         <v>46.50334192</v>
       </c>
       <c r="S2">
-        <v>56.53109005</v>
+        <v>53.89737328</v>
       </c>
       <c r="T2">
-        <v>68.72117165</v>
+        <v>62.46705563</v>
       </c>
       <c r="U2">
-        <v>83.5398615</v>
+        <v>72.39931747999999</v>
       </c>
       <c r="V2">
-        <v>101.5539795</v>
+        <v>83.91080896</v>
       </c>
       <c r="W2">
-        <v>123.4525719</v>
+        <v>97.25262758</v>
       </c>
       <c r="X2">
-        <v>150.0732673</v>
+        <v>112.7157954</v>
       </c>
       <c r="Y2">
-        <v>182.4343162</v>
+        <v>130.6376068</v>
       </c>
       <c r="Z2">
-        <v>199.2018542</v>
+        <v>140.0435145</v>
       </c>
       <c r="AA2">
-        <v>217.5104967</v>
+        <v>150.1266476</v>
       </c>
       <c r="AB2">
-        <v>237.5018864</v>
+        <v>160.9357662</v>
       </c>
       <c r="AC2">
-        <v>259.3306848</v>
+        <v>172.5231414</v>
       </c>
       <c r="AD2">
-        <v>283.165768</v>
+        <v>184.9448075</v>
       </c>
       <c r="AE2">
-        <v>321.6038221</v>
+        <v>199.3705025</v>
       </c>
       <c r="AF2">
-        <v>365.2596113</v>
+        <v>214.9214017</v>
       </c>
       <c r="AG2">
-        <v>414.841412</v>
+        <v>231.6852711</v>
       </c>
       <c r="AH2">
-        <v>471.1536446</v>
+        <v>249.7567222</v>
       </c>
       <c r="AI2">
-        <v>535.1099249</v>
+        <v>269.2377465</v>
       </c>
       <c r="AJ2">
-        <v>584.2918781</v>
+        <v>292.3921927</v>
       </c>
       <c r="AK2">
-        <v>637.9941446</v>
+        <v>317.5379213</v>
       </c>
       <c r="AL2">
-        <v>696.6321865</v>
+        <v>344.8461825</v>
       </c>
       <c r="AM2">
-        <v>760.6596507</v>
+        <v>374.5029542</v>
       </c>
       <c r="AN2">
-        <v>830.5718792</v>
+        <v>406.7102083</v>
       </c>
       <c r="AO2">
-        <v>912.1946695</v>
+        <v>443.314127</v>
       </c>
       <c r="AP2">
-        <v>1001.838776</v>
+        <v>483.2123985</v>
       </c>
       <c r="AQ2">
-        <v>1100.292478</v>
+        <v>526.7015143</v>
       </c>
       <c r="AR2">
-        <v>1208.421521</v>
+        <v>574.1046506</v>
       </c>
       <c r="AS2">
-        <v>1327.176729</v>
+        <v>625.7740692</v>
       </c>
     </row>
     <row r="3" spans="1:45">

</xml_diff>